<commit_message>
translation table between wrds&refinitiv
</commit_message>
<xml_diff>
--- a/files/tl_table/basic_param_tl_table.xlsx
+++ b/files/tl_table/basic_param_tl_table.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesd/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djwja\GitHub\eikonproj\files\tl_table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{518EFFA5-E535-C846-8A91-2D0BB2AF11E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B1CFA2-1680-4985-8C90-3F7A67439865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{95991D6C-D455-ED48-A11F-706F5563326E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{95991D6C-D455-ED48-A11F-706F5563326E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="295">
   <si>
     <t>funda</t>
   </si>
@@ -752,12 +753,6 @@
     <t>TR.EBITActValue</t>
   </si>
   <si>
-    <t>TR.InterestIncomeNoneOperating+TR.OtherNonOperatingIncome</t>
-  </si>
-  <si>
-    <t>-TR.SpecialItems</t>
-  </si>
-  <si>
     <t>TR.NetIncomeBeforeTaxes</t>
   </si>
   <si>
@@ -888,18 +883,86 @@
   </si>
   <si>
     <t>else: TR.BankTotalRevenue</t>
+  </si>
+  <si>
+    <t>TR.BankTotalRevenue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR.TotalInterestExpense</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR.LaborRelatedExpense</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR.EBITDA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR.EBIT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR.InterestIncomeNonOperating+TR.OtherNonOperatingIncome</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR.SpecialItemsMM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR.InterestExpense</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR.OtherEarningAssetsTotal-TR.TradingAccountAssets</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR.TradingAccountAssets+TR.TotalInvestmentSecurities</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR.OtherLTAssetsTotal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sale</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR.IntExpenseNetNonOper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -943,16 +1006,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -968,7 +1030,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1266,23 +1328,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E66578-90B9-E344-AC73-460374EDFAF0}">
   <dimension ref="A1:V95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="E43" zoomScale="138" workbookViewId="0">
+      <selection activeCell="T62" sqref="T62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="8.33203125" customWidth="1"/>
     <col min="8" max="18" width="8.33203125" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="19" max="19" width="36" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E1" t="s">
         <v>62</v>
       </c>
@@ -1313,7 +1375,7 @@
       <c r="N1" t="s">
         <v>206</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>220</v>
       </c>
       <c r="P1" t="s">
@@ -1332,7 +1394,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>95</v>
       </c>
@@ -1346,7 +1408,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1365,14 +1427,14 @@
       <c r="G3">
         <v>60530</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="S3" t="s">
         <v>131</v>
       </c>
       <c r="T3" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -1385,17 +1447,17 @@
       <c r="G4">
         <v>60530</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="S4" t="s">
         <v>131</v>
       </c>
       <c r="T4" t="s">
         <v>229</v>
       </c>
       <c r="V4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>4</v>
       </c>
@@ -1412,10 +1474,10 @@
         <v>230</v>
       </c>
       <c r="V5" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
         <v>5</v>
       </c>
@@ -1435,7 +1497,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>6</v>
       </c>
@@ -1452,7 +1514,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
         <v>7</v>
       </c>
@@ -1472,8 +1534,8 @@
         <v>233</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="D9" t="s">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="D9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E9" t="s">
@@ -1492,7 +1554,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>9</v>
       </c>
@@ -1505,14 +1567,14 @@
       <c r="G10">
         <v>1783</v>
       </c>
-      <c r="S10" s="1" t="s">
+      <c r="S10" t="s">
         <v>139</v>
       </c>
       <c r="T10" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>10</v>
       </c>
@@ -1525,14 +1587,14 @@
       <c r="G11">
         <v>12677</v>
       </c>
-      <c r="S11" s="1" t="s">
+      <c r="S11" t="s">
         <v>135</v>
       </c>
       <c r="T11" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>111</v>
       </c>
@@ -1552,7 +1614,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>11</v>
       </c>
@@ -1566,10 +1628,10 @@
         <v>484</v>
       </c>
       <c r="T13" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>12</v>
       </c>
@@ -1588,11 +1650,11 @@
       <c r="L14">
         <v>-1753</v>
       </c>
-      <c r="T14" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="T14" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>13</v>
       </c>
@@ -1609,10 +1671,10 @@
         <v>124</v>
       </c>
       <c r="T15" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>14</v>
       </c>
@@ -1638,11 +1700,11 @@
         <v>3.5</v>
       </c>
       <c r="T16" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="17" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="D17" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="D17" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E17" t="s">
@@ -1654,15 +1716,15 @@
       <c r="G17">
         <v>1639</v>
       </c>
-      <c r="S17" s="1" t="s">
+      <c r="S17" t="s">
         <v>136</v>
       </c>
       <c r="T17" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="18" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="D18" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="18" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="D18" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E18" t="s">
@@ -1675,8 +1737,8 @@
         <v>391</v>
       </c>
     </row>
-    <row r="19" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="D19" t="s">
+    <row r="19" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="D19" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E19" t="s">
@@ -1689,7 +1751,7 @@
         <v>1677</v>
       </c>
     </row>
-    <row r="20" spans="3:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:20" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>18</v>
       </c>
@@ -1706,10 +1768,10 @@
         <v>137</v>
       </c>
       <c r="T20" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="21" spans="3:20" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="21" spans="3:20" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>19</v>
       </c>
@@ -1725,11 +1787,11 @@
       <c r="S21" t="s">
         <v>138</v>
       </c>
-      <c r="T21" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="22" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="T21" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="22" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>20</v>
       </c>
@@ -1745,14 +1807,14 @@
       <c r="G22">
         <v>1346</v>
       </c>
-      <c r="S22" s="2" t="s">
+      <c r="S22" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="T22" s="2" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="23" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="T22" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="23" spans="3:20" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>22</v>
       </c>
@@ -1769,10 +1831,10 @@
         <v>164</v>
       </c>
       <c r="T23" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="24" spans="3:20" x14ac:dyDescent="0.2">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="24" spans="3:20" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>23</v>
       </c>
@@ -1789,11 +1851,11 @@
         <v>165</v>
       </c>
       <c r="T24" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="25" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="D25" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="25" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="D25" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E25" t="s">
@@ -1809,11 +1871,11 @@
         <v>404381</v>
       </c>
       <c r="T25" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="26" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="D26" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="26" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="D26" s="4" t="s">
         <v>140</v>
       </c>
       <c r="E26" t="s">
@@ -1832,8 +1894,8 @@
         <v>60.305</v>
       </c>
     </row>
-    <row r="27" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="D27" t="s">
+    <row r="27" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="D27" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E27" t="s">
@@ -1852,8 +1914,8 @@
         <v>92.777000000000001</v>
       </c>
     </row>
-    <row r="28" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="D28" t="s">
+    <row r="28" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="D28" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E28" t="s">
@@ -1869,7 +1931,7 @@
         <v>460.9</v>
       </c>
     </row>
-    <row r="29" spans="3:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
         <v>27</v>
       </c>
@@ -1885,14 +1947,14 @@
       <c r="G29">
         <v>15611</v>
       </c>
-      <c r="S29" s="3" t="s">
+      <c r="S29" s="2" t="s">
         <v>166</v>
       </c>
       <c r="T29" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="30" spans="3:20" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="30" spans="3:20" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
         <v>29</v>
       </c>
@@ -1909,10 +1971,10 @@
         <v>167</v>
       </c>
       <c r="T30" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="31" spans="3:20" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="31" spans="3:20" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
         <v>30</v>
       </c>
@@ -1929,10 +1991,10 @@
         <v>168</v>
       </c>
       <c r="T31" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="32" spans="3:20" x14ac:dyDescent="0.2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="32" spans="3:20" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
         <v>31</v>
       </c>
@@ -1945,12 +2007,12 @@
       <c r="G32">
         <v>21573</v>
       </c>
-      <c r="S32" s="4"/>
+      <c r="S32" s="3"/>
       <c r="T32" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="33" spans="3:22" x14ac:dyDescent="0.2">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="33" spans="3:22" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
         <v>32</v>
       </c>
@@ -1963,17 +2025,17 @@
       <c r="G33">
         <v>1552</v>
       </c>
-      <c r="S33" s="5" t="s">
+      <c r="S33" t="s">
         <v>169</v>
       </c>
       <c r="T33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="U33" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="34" spans="3:22" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="34" spans="3:22" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
         <v>33</v>
       </c>
@@ -1986,14 +2048,14 @@
       <c r="G34">
         <v>127243</v>
       </c>
-      <c r="S34" s="5" t="s">
+      <c r="S34" t="s">
         <v>170</v>
       </c>
       <c r="T34" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="35" spans="3:22" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="35" spans="3:22" x14ac:dyDescent="0.3">
       <c r="D35" t="s">
         <v>34</v>
       </c>
@@ -2006,14 +2068,14 @@
       <c r="G35">
         <v>3114</v>
       </c>
-      <c r="S35" s="5" t="s">
+      <c r="S35" t="s">
         <v>171</v>
       </c>
       <c r="T35" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="36" spans="3:22" x14ac:dyDescent="0.2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="36" spans="3:22" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
         <v>35</v>
       </c>
@@ -2032,14 +2094,14 @@
       <c r="K36">
         <v>846.30600000000004</v>
       </c>
-      <c r="S36" s="5" t="s">
+      <c r="S36" t="s">
         <v>172</v>
       </c>
       <c r="T36" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="37" spans="3:22" x14ac:dyDescent="0.2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="37" spans="3:22" x14ac:dyDescent="0.3">
       <c r="D37" t="s">
         <v>36</v>
       </c>
@@ -2053,10 +2115,10 @@
         <v>16802</v>
       </c>
       <c r="T37" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="38" spans="3:22" x14ac:dyDescent="0.2">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="38" spans="3:22" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
         <v>37</v>
       </c>
@@ -2073,10 +2135,10 @@
         <v>173</v>
       </c>
       <c r="T38" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="39" spans="3:22" x14ac:dyDescent="0.2">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="39" spans="3:22" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
         <v>207</v>
       </c>
@@ -2093,10 +2155,10 @@
         <v>158</v>
       </c>
       <c r="T39" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="40" spans="3:22" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="40" spans="3:22" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
         <v>38</v>
       </c>
@@ -2119,10 +2181,10 @@
         <v>174</v>
       </c>
       <c r="T40" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="41" spans="3:22" x14ac:dyDescent="0.2">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="41" spans="3:22" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
         <v>39</v>
       </c>
@@ -2136,10 +2198,10 @@
         <v>2878</v>
       </c>
       <c r="T41" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="42" spans="3:22" x14ac:dyDescent="0.2">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="42" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
         <v>40</v>
       </c>
@@ -2159,10 +2221,10 @@
         <v>190</v>
       </c>
       <c r="T42" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="43" spans="3:22" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="43" spans="3:22" x14ac:dyDescent="0.3">
       <c r="D43" t="s">
         <v>42</v>
       </c>
@@ -2179,10 +2241,10 @@
         <v>194</v>
       </c>
       <c r="T43" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="44" spans="3:22" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="44" spans="3:22" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
         <v>43</v>
       </c>
@@ -2199,10 +2261,10 @@
         <v>195</v>
       </c>
       <c r="T44" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="45" spans="3:22" x14ac:dyDescent="0.2">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="45" spans="3:22" x14ac:dyDescent="0.3">
       <c r="D45" t="s">
         <v>44</v>
       </c>
@@ -2219,11 +2281,11 @@
         <v>191</v>
       </c>
       <c r="T45" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="46" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="D46" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="46" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="D46" s="4" t="s">
         <v>45</v>
       </c>
       <c r="E46" t="s">
@@ -2245,11 +2307,11 @@
         <v>23791</v>
       </c>
       <c r="T46" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="47" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="D47" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="47" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="D47" s="4" t="s">
         <v>46</v>
       </c>
       <c r="E47" t="s">
@@ -2271,14 +2333,14 @@
         <v>3742.52</v>
       </c>
       <c r="T47" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="V47" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="48" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="D48" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="48" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="D48" s="4" t="s">
         <v>47</v>
       </c>
       <c r="E48" t="s">
@@ -2318,8 +2380,8 @@
         <v>148</v>
       </c>
     </row>
-    <row r="49" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="D49" t="s">
+    <row r="49" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="D49" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E49" t="s">
@@ -2341,10 +2403,10 @@
         <v>3742.52</v>
       </c>
       <c r="T49" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="50" spans="2:20" x14ac:dyDescent="0.2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="50" spans="2:20" x14ac:dyDescent="0.3">
       <c r="D50" t="s">
         <v>49</v>
       </c>
@@ -2364,10 +2426,10 @@
         <v>11253</v>
       </c>
       <c r="T50" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="51" spans="2:20" x14ac:dyDescent="0.2">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="51" spans="2:20" x14ac:dyDescent="0.3">
       <c r="D51" t="s">
         <v>50</v>
       </c>
@@ -2384,10 +2446,10 @@
         <v>192</v>
       </c>
       <c r="T51" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="52" spans="2:20" x14ac:dyDescent="0.2">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="52" spans="2:20" x14ac:dyDescent="0.3">
       <c r="D52" t="s">
         <v>51</v>
       </c>
@@ -2401,10 +2463,10 @@
         <v>19625</v>
       </c>
       <c r="T52" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="53" spans="2:20" x14ac:dyDescent="0.2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="53" spans="2:20" x14ac:dyDescent="0.3">
       <c r="D53" t="s">
         <v>52</v>
       </c>
@@ -2418,11 +2480,11 @@
         <v>23046</v>
       </c>
       <c r="T53" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="54" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="D54" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="54" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="D54" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E54" t="s">
@@ -2438,11 +2500,11 @@
         <v>193</v>
       </c>
       <c r="T54" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="55" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="D55" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="55" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="D55" s="4" t="s">
         <v>54</v>
       </c>
       <c r="E55" t="s">
@@ -2458,10 +2520,10 @@
         <v>196</v>
       </c>
       <c r="T55" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="56" spans="2:20" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="56" spans="2:20" x14ac:dyDescent="0.3">
       <c r="D56" t="s">
         <v>55</v>
       </c>
@@ -2475,10 +2537,10 @@
         <v>-2879</v>
       </c>
       <c r="T56" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="57" spans="2:20" x14ac:dyDescent="0.2">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="57" spans="2:20" x14ac:dyDescent="0.3">
       <c r="D57" t="s">
         <v>56</v>
       </c>
@@ -2492,11 +2554,11 @@
         <v>21944</v>
       </c>
       <c r="T57" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="58" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="D58" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="58" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="D58" s="4" t="s">
         <v>57</v>
       </c>
       <c r="E58" t="s">
@@ -2506,10 +2568,10 @@
         <v>148</v>
       </c>
       <c r="T58" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="59" spans="2:20" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="59" spans="2:20" x14ac:dyDescent="0.3">
       <c r="D59" t="s">
         <v>58</v>
       </c>
@@ -2523,11 +2585,11 @@
         <v>288.3</v>
       </c>
       <c r="T59" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="60" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="D60" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="60" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="D60" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E60" t="s">
@@ -2539,15 +2601,15 @@
       <c r="G60">
         <v>906.09199999999998</v>
       </c>
-      <c r="T60" s="2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="61" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="T60" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="61" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C61" t="s">
         <v>60</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="4" t="s">
         <v>61</v>
       </c>
       <c r="E61" t="s">
@@ -2559,11 +2621,11 @@
       <c r="G61">
         <v>140.88999999999999</v>
       </c>
-      <c r="T61" s="2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="62" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="T61" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="62" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>91</v>
       </c>
@@ -2577,7 +2639,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="63" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>65</v>
       </c>
@@ -2597,7 +2659,7 @@
         <v>2870</v>
       </c>
     </row>
-    <row r="64" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:20" x14ac:dyDescent="0.3">
       <c r="D64" t="s">
         <v>67</v>
       </c>
@@ -2611,7 +2673,7 @@
         <v>16690</v>
       </c>
     </row>
-    <row r="65" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D65" t="s">
         <v>68</v>
       </c>
@@ -2625,7 +2687,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="66" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D66" t="s">
         <v>69</v>
       </c>
@@ -2639,7 +2701,7 @@
         <v>16690</v>
       </c>
     </row>
-    <row r="67" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D67" t="s">
         <v>70</v>
       </c>
@@ -2653,7 +2715,7 @@
         <v>6091</v>
       </c>
     </row>
-    <row r="68" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D68" t="s">
         <v>71</v>
       </c>
@@ -2667,7 +2729,7 @@
         <v>6108</v>
       </c>
     </row>
-    <row r="69" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C69" t="s">
         <v>78</v>
       </c>
@@ -2684,7 +2746,7 @@
         <v>127243</v>
       </c>
     </row>
-    <row r="70" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D70" t="s">
         <v>73</v>
       </c>
@@ -2698,7 +2760,7 @@
         <v>29118</v>
       </c>
     </row>
-    <row r="71" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="71" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D71" t="s">
         <v>74</v>
       </c>
@@ -2712,7 +2774,7 @@
         <v>8841</v>
       </c>
     </row>
-    <row r="72" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D72" t="s">
         <v>75</v>
       </c>
@@ -2726,7 +2788,7 @@
         <v>31505</v>
       </c>
     </row>
-    <row r="73" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="73" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D73" t="s">
         <v>76</v>
       </c>
@@ -2740,7 +2802,7 @@
         <v>5633</v>
       </c>
     </row>
-    <row r="74" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="74" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D74" t="s">
         <v>77</v>
       </c>
@@ -2754,11 +2816,11 @@
         <v>8212</v>
       </c>
     </row>
-    <row r="75" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="75" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C75" t="s">
         <v>79</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="4" t="s">
         <v>80</v>
       </c>
       <c r="E75" t="s">
@@ -2768,8 +2830,8 @@
         <v>138.19999999999999</v>
       </c>
     </row>
-    <row r="76" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="D76" t="s">
+    <row r="76" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="D76" s="4" t="s">
         <v>212</v>
       </c>
       <c r="E76" t="s">
@@ -2779,7 +2841,7 @@
         <v>15943.424999999999</v>
       </c>
     </row>
-    <row r="77" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="77" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D77" t="s">
         <v>81</v>
       </c>
@@ -2790,7 +2852,7 @@
         <v>50672</v>
       </c>
     </row>
-    <row r="78" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="78" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D78" t="s">
         <v>82</v>
       </c>
@@ -2801,8 +2863,8 @@
         <v>50672</v>
       </c>
     </row>
-    <row r="79" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="D79" t="s">
+    <row r="79" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="D79" s="4" t="s">
         <v>83</v>
       </c>
       <c r="E79" t="s">
@@ -2818,7 +2880,7 @@
         <v>2935</v>
       </c>
     </row>
-    <row r="80" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="80" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D80" t="s">
         <v>84</v>
       </c>
@@ -2835,8 +2897,8 @@
         <v>2512</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="D81" t="s">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="D81" s="4" t="s">
         <v>85</v>
       </c>
       <c r="E81" t="s">
@@ -2846,7 +2908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>96</v>
       </c>
@@ -2857,17 +2919,17 @@
         <v>86</v>
       </c>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D83" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D84" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D85" t="s">
         <v>89</v>
       </c>
@@ -2875,17 +2937,17 @@
         <v>90</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D86" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D87" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>100</v>
       </c>
@@ -2899,7 +2961,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D89" t="s">
         <v>103</v>
       </c>
@@ -2907,7 +2969,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D90" t="s">
         <v>104</v>
       </c>
@@ -2915,7 +2977,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D91" t="s">
         <v>105</v>
       </c>
@@ -2923,7 +2985,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D92" t="s">
         <v>106</v>
       </c>
@@ -2931,7 +2993,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D93" t="s">
         <v>107</v>
       </c>
@@ -2939,7 +3001,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D94" t="s">
         <v>109</v>
       </c>
@@ -2947,7 +3009,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D95" t="s">
         <v>108</v>
       </c>
@@ -2956,9 +3018,670 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="O1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0C46C0B-BF70-45E0-AC6A-657774F3F26A}">
+  <dimension ref="A1:C93"/>
+  <sheetViews>
+    <sheetView zoomScale="163" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>231</v>
+      </c>
+      <c r="C4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>294</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" t="s">
+        <v>248</v>
+      </c>
+      <c r="C27" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
+        <v>250</v>
+      </c>
+      <c r="C29" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
+        <v>252</v>
+      </c>
+      <c r="C31" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>207</v>
+      </c>
+      <c r="B37" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>